<commit_message>
Commit 10: Employee, Department, WorkingTime comps
</commit_message>
<xml_diff>
--- a/Development Phases.xlsx
+++ b/Development Phases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\TimeSheetApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060F7C06-FB8C-4FA1-A00C-5513B6899ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83693AD4-592A-478D-9E49-7AA756CD22DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8E109C7E-A975-45C7-B039-39425A8BA5F1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
   <si>
     <t>R.B</t>
   </si>
@@ -118,6 +118,24 @@
   </si>
   <si>
     <t>Item elements - CompanyItem, CompanyList, CompanyDetails</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loading sa backend-a za company </t>
+  </si>
+  <si>
+    <t>Loading sa backend-a za department</t>
+  </si>
+  <si>
+    <t>Prikaz za department na frontend-u</t>
+  </si>
+  <si>
+    <t>Prikaz za company na frontend-u</t>
+  </si>
+  <si>
+    <t>Loading sa backend-a za employee</t>
+  </si>
+  <si>
+    <t>Prikaz za employees na frontend-u</t>
   </si>
 </sst>
 </file>
@@ -561,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2929433E-857F-40DE-B57B-B06575538643}">
-  <dimension ref="C2:E29"/>
+  <dimension ref="C2:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,24 +870,90 @@
       </c>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C28" s="7">
+      <c r="C28" s="2">
         <v>12</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="7">
+      <c r="C29" s="2">
         <v>13</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C30" s="2">
+        <v>14.1</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C31" s="2">
+        <v>14.2</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C32" s="2">
+        <v>15.1</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C33" s="2">
+        <v>15.2</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34" s="2">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C35" s="7">
+        <v>16.2</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="8" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit 11: filtering added
</commit_message>
<xml_diff>
--- a/Development Phases.xlsx
+++ b/Development Phases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\TimeSheetApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83693AD4-592A-478D-9E49-7AA756CD22DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F0A1BD-CE2A-42F2-A70E-38202690B0AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8E109C7E-A975-45C7-B039-39425A8BA5F1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
   <si>
     <t>R.B</t>
   </si>
@@ -136,6 +136,15 @@
   </si>
   <si>
     <t>Prikaz za employees na frontend-u</t>
+  </si>
+  <si>
+    <t>Loading sa backend-a za workingtimes</t>
+  </si>
+  <si>
+    <t>Prikaz za workingtimes na frontend-u</t>
+  </si>
+  <si>
+    <t>Employee filtering added</t>
   </si>
 </sst>
 </file>
@@ -579,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2929433E-857F-40DE-B57B-B06575538643}">
-  <dimension ref="C2:E35"/>
+  <dimension ref="C2:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38:E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,13 +956,46 @@
       </c>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C35" s="7">
+      <c r="C35" s="2">
         <v>16.2</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C36" s="2">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C37" s="2">
+        <v>17.2</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C38" s="7">
+        <v>18</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E38" s="8" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit 12: Create i Update za Company i Department
</commit_message>
<xml_diff>
--- a/Development Phases.xlsx
+++ b/Development Phases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\TimeSheetApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F0A1BD-CE2A-42F2-A70E-38202690B0AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71110A04-6C48-4E9D-9A37-8096BF6A05A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8E109C7E-A975-45C7-B039-39425A8BA5F1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="44">
   <si>
     <t>R.B</t>
   </si>
@@ -144,7 +144,19 @@
     <t>Prikaz za workingtimes na frontend-u</t>
   </si>
   <si>
-    <t>Employee filtering added</t>
+    <t>Employee and WorkingTimes filtering added</t>
+  </si>
+  <si>
+    <t>Dinamičko mijenjanje linkova u header-u</t>
+  </si>
+  <si>
+    <t>Forme za kreiranje company, employee i department</t>
+  </si>
+  <si>
+    <t>Create i Update za company</t>
+  </si>
+  <si>
+    <t>Create i Update za department</t>
   </si>
 </sst>
 </file>
@@ -588,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2929433E-857F-40DE-B57B-B06575538643}">
-  <dimension ref="C2:E38"/>
+  <dimension ref="C2:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38:E38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41:E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,13 +1001,57 @@
       </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C38" s="7">
-        <v>18</v>
-      </c>
-      <c r="D38" s="8" t="s">
+      <c r="C38" s="2">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E38" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C39" s="7">
+        <v>18.2</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C40" s="7">
+        <v>19</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C41" s="7">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C42" s="7">
+        <v>20.2</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E42" s="8" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit 15: Delete com, emp, dep, wt
</commit_message>
<xml_diff>
--- a/Development Phases.xlsx
+++ b/Development Phases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\TimeSheetApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71110A04-6C48-4E9D-9A37-8096BF6A05A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826419EC-2541-4028-A8BD-54EB9A5D6E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8E109C7E-A975-45C7-B039-39425A8BA5F1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="49">
   <si>
     <t>R.B</t>
   </si>
@@ -157,6 +157,21 @@
   </si>
   <si>
     <t>Create i Update za department</t>
+  </si>
+  <si>
+    <t>Create i Update za employee</t>
+  </si>
+  <si>
+    <t>Loading Spinner</t>
+  </si>
+  <si>
+    <t>BaseDialog for errors</t>
+  </si>
+  <si>
+    <t>Route transition</t>
+  </si>
+  <si>
+    <t>NotFound page</t>
   </si>
 </sst>
 </file>
@@ -600,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2929433E-857F-40DE-B57B-B06575538643}">
-  <dimension ref="C2:E42"/>
+  <dimension ref="C2:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41:E42"/>
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,46 +1027,101 @@
       </c>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C39" s="7">
+      <c r="C39" s="2">
         <v>18.2</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="E39" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C40" s="7">
+      <c r="C40" s="2">
         <v>19</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="E40" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="7">
+      <c r="C41" s="2">
         <v>20.100000000000001</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E41" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C42" s="7">
+      <c r="C42" s="2">
         <v>20.2</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D42" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="E42" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C43" s="7">
+        <v>20.3</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C44" s="7">
+        <v>21</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C45" s="7">
+        <v>22</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C46" s="7">
+        <v>23</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C47" s="7">
+        <v>24</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E47" s="8" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit 17: Statistics full done
</commit_message>
<xml_diff>
--- a/Development Phases.xlsx
+++ b/Development Phases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\TimeSheetApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEA1018-7D3C-439A-9D95-2110AFCF6535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0207A8-4C46-4B8A-AE33-69BA5EB0993B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8E109C7E-A975-45C7-B039-39425A8BA5F1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="57">
   <si>
     <t>R.B</t>
   </si>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>Statistic Component</t>
+  </si>
+  <si>
+    <t>Create, Edit, Delete for Auth</t>
+  </si>
+  <si>
+    <t>Statistic filter</t>
   </si>
 </sst>
 </file>
@@ -262,7 +268,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2929433E-857F-40DE-B57B-B06575538643}">
-  <dimension ref="C2:F51"/>
+  <dimension ref="C2:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,25 +1260,52 @@
       <c r="D49" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E49" s="1"/>
+      <c r="E49" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F49" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="50" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
-        <v>29</v>
+        <v>29.1</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E50" s="1"/>
+      <c r="E50" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F50" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="51" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C51" s="4"/>
+      <c r="C51" s="2">
+        <v>29.2</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C52" s="2">
+        <v>30</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E52" s="1"/>
+      <c r="F52" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Commit 18: Auth frontend, requests and controllers
</commit_message>
<xml_diff>
--- a/Development Phases.xlsx
+++ b/Development Phases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\TimeSheetApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0207A8-4C46-4B8A-AE33-69BA5EB0993B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0FF2C9-05B6-41DC-95B2-327B123A6AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8E109C7E-A975-45C7-B039-39425A8BA5F1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="65">
   <si>
     <t>R.B</t>
   </si>
@@ -192,10 +192,34 @@
     <t>Statistic Component</t>
   </si>
   <si>
-    <t>Create, Edit, Delete for Auth</t>
-  </si>
-  <si>
     <t>Statistic filter</t>
+  </si>
+  <si>
+    <t>Create, Edit for Auth</t>
+  </si>
+  <si>
+    <t>Login Method</t>
+  </si>
+  <si>
+    <t>Correcting every method and form</t>
+  </si>
+  <si>
+    <t>Adapting every request for token auth</t>
+  </si>
+  <si>
+    <t>GenerateController</t>
+  </si>
+  <si>
+    <t>Generate Component</t>
+  </si>
+  <si>
+    <t>Router - AuthGuards</t>
+  </si>
+  <si>
+    <t>Backend controllers</t>
+  </si>
+  <si>
+    <t>About page and documentation</t>
   </si>
 </sst>
 </file>
@@ -263,11 +287,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -583,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2929433E-857F-40DE-B57B-B06575538643}">
-  <dimension ref="C2:F52"/>
+  <dimension ref="C2:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,7 +1311,7 @@
         <v>29.2</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>5</v>
@@ -1299,11 +1324,119 @@
       <c r="C52" s="2">
         <v>30</v>
       </c>
-      <c r="D52" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E52" s="1"/>
-      <c r="F52" s="4" t="s">
+      <c r="D52" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C53" s="2">
+        <v>31.1</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C54" s="2">
+        <v>31.2</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C55" s="2">
+        <v>32</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C56" s="2">
+        <v>33</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C57" s="2">
+        <v>34</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C58" s="2">
+        <v>35</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C59" s="2">
+        <v>36</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C60" s="4">
+        <v>37</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E60" s="1"/>
+      <c r="F60" s="5" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit 19: Emp filter, EditUser, Random Data Gen
</commit_message>
<xml_diff>
--- a/Development Phases.xlsx
+++ b/Development Phases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\TimeSheetApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0FF2C9-05B6-41DC-95B2-327B123A6AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F980A771-433F-40CD-87DB-35EC56FB465B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8E109C7E-A975-45C7-B039-39425A8BA5F1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="68">
   <si>
     <t>R.B</t>
   </si>
@@ -220,6 +220,15 @@
   </si>
   <si>
     <t>About page and documentation</t>
+  </si>
+  <si>
+    <t>Edit User page</t>
+  </si>
+  <si>
+    <t>Final testings</t>
+  </si>
+  <si>
+    <t>Backend/Frontend</t>
   </si>
 </sst>
 </file>
@@ -608,16 +617,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2929433E-857F-40DE-B57B-B06575538643}">
-  <dimension ref="C2:F60"/>
+  <dimension ref="C2:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="5.140625" customWidth="1"/>
     <col min="4" max="4" width="104.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:6" ht="21" x14ac:dyDescent="0.35">
@@ -1411,7 +1421,9 @@
       <c r="D58" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E58" s="1"/>
+      <c r="E58" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F58" s="1" t="s">
         <v>23</v>
       </c>
@@ -1423,21 +1435,49 @@
       <c r="D59" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E59" s="1"/>
+      <c r="E59" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F59" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="60" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C60" s="4">
+      <c r="C60" s="2">
         <v>37</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C61" s="4">
+        <v>38</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E60" s="1"/>
-      <c r="F60" s="5" t="s">
-        <v>25</v>
+      <c r="E61" s="1"/>
+      <c r="F61" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C62" s="4">
+        <v>39</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E62" s="1"/>
+      <c r="F62" s="5" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit 20: final touches
</commit_message>
<xml_diff>
--- a/Development Phases.xlsx
+++ b/Development Phases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\TimeSheetApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F980A771-433F-40CD-87DB-35EC56FB465B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47F5309-B492-451A-9026-F3992B5DDC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8E109C7E-A975-45C7-B039-39425A8BA5F1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="68">
   <si>
     <t>R.B</t>
   </si>
@@ -296,13 +296,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,7 +618,7 @@
   <dimension ref="C2:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1457,26 +1455,30 @@
       </c>
     </row>
     <row r="61" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C61" s="4">
+      <c r="C61" s="2">
         <v>38</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E61" s="1"/>
-      <c r="F61" s="5" t="s">
+      <c r="E61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="62" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C62" s="4">
+      <c r="C62" s="2">
         <v>39</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E62" s="1"/>
-      <c r="F62" s="5" t="s">
+      <c r="E62" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F62" s="1" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>